<commit_message>
🔧 Save current state before security fixes
- Updated step3_data_mapping.py with F/M/C logic fixes
- Updated common/config.py with new column mappings
- Added TP REGNBROM original test file

✨ Pipeline now successfully processes F/M/C sheet types
🎯 Generated with Claude Code
</commit_message>
<xml_diff>
--- a/input/Test plan SLÅTTERVALL ver  2.xlsx
+++ b/input/Test plan SLÅTTERVALL ver  2.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/truongxuantruong/Desktop/Ngoc Son internal TSS converter/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5A2B24-F26C-3B4D-8784-EB428C133B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64A86F2-190C-B644-8B34-3E7BFCAB149A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Finished product" sheetId="2" r:id="rId1"/>
-    <sheet name="Textile" sheetId="4" r:id="rId2"/>
+    <sheet name="F-Finished product" sheetId="2" r:id="rId1"/>
+    <sheet name="M-Textile" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Finished product'!$A$19:$AK$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Textile!$A$20:$AN$316</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'F-Finished product'!$A$19:$AK$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'M-Textile'!$A$20:$AN$316</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3324,6 +3324,78 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="2" borderId="12" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="2" borderId="13" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="2" borderId="14" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3333,76 +3405,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="2" borderId="12" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="2" borderId="13" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="2" borderId="14" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3451,12 +3457,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4004,7 +4004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="73" zoomScaleNormal="73" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A8" zoomScale="73" zoomScaleNormal="73" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A12" sqref="A12"/>
       <selection pane="topRight" activeCell="E23" sqref="E23"/>
@@ -4079,10 +4079,10 @@
       <c r="V1" s="4"/>
       <c r="W1" s="5"/>
       <c r="X1" s="2"/>
-      <c r="Y1" s="304" t="s">
+      <c r="Y1" s="319" t="s">
         <v>1</v>
       </c>
-      <c r="Z1" s="305"/>
+      <c r="Z1" s="320"/>
       <c r="AA1" s="6"/>
       <c r="AB1" s="6"/>
       <c r="AC1" s="7"/>
@@ -4090,11 +4090,11 @@
         <f t="shared" ref="AE1:AJ19" si="0">IF(X1&lt;&gt;"",X1,"")</f>
         <v/>
       </c>
-      <c r="AF1" s="304" t="str">
+      <c r="AF1" s="319" t="str">
         <f t="shared" si="0"/>
         <v>Mã số: BM-KĐ-14</v>
       </c>
-      <c r="AG1" s="305" t="str">
+      <c r="AG1" s="320" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4136,10 +4136,10 @@
       <c r="V2" s="13"/>
       <c r="W2" s="14"/>
       <c r="X2" s="11"/>
-      <c r="Y2" s="306" t="s">
+      <c r="Y2" s="321" t="s">
         <v>2</v>
       </c>
-      <c r="Z2" s="307"/>
+      <c r="Z2" s="322"/>
       <c r="AA2" s="15"/>
       <c r="AB2" s="15"/>
       <c r="AC2" s="7"/>
@@ -4147,11 +4147,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AF2" s="306" t="str">
+      <c r="AF2" s="321" t="str">
         <f t="shared" si="0"/>
         <v>Ngày ban hành: 01/7/2015</v>
       </c>
-      <c r="AG2" s="307" t="str">
+      <c r="AG2" s="322" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4170,28 +4170,28 @@
     </row>
     <row r="3" spans="1:36" ht="17.25" customHeight="1">
       <c r="A3" s="10"/>
-      <c r="B3" s="308" t="s">
+      <c r="B3" s="323" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="308"/>
-      <c r="D3" s="308"/>
-      <c r="E3" s="308"/>
-      <c r="F3" s="308"/>
-      <c r="G3" s="308"/>
-      <c r="H3" s="308"/>
-      <c r="I3" s="308"/>
-      <c r="J3" s="308"/>
-      <c r="K3" s="308"/>
-      <c r="L3" s="308"/>
-      <c r="M3" s="308"/>
-      <c r="N3" s="308"/>
-      <c r="O3" s="308"/>
-      <c r="P3" s="308"/>
-      <c r="Q3" s="308"/>
-      <c r="R3" s="308"/>
-      <c r="S3" s="308"/>
-      <c r="T3" s="308"/>
-      <c r="U3" s="308"/>
+      <c r="C3" s="323"/>
+      <c r="D3" s="323"/>
+      <c r="E3" s="323"/>
+      <c r="F3" s="323"/>
+      <c r="G3" s="323"/>
+      <c r="H3" s="323"/>
+      <c r="I3" s="323"/>
+      <c r="J3" s="323"/>
+      <c r="K3" s="323"/>
+      <c r="L3" s="323"/>
+      <c r="M3" s="323"/>
+      <c r="N3" s="323"/>
+      <c r="O3" s="323"/>
+      <c r="P3" s="323"/>
+      <c r="Q3" s="323"/>
+      <c r="R3" s="323"/>
+      <c r="S3" s="323"/>
+      <c r="T3" s="323"/>
+      <c r="U3" s="323"/>
       <c r="V3" s="151"/>
       <c r="W3" s="17"/>
       <c r="X3" s="18"/>
@@ -4229,26 +4229,26 @@
     </row>
     <row r="4" spans="1:36" ht="15" customHeight="1">
       <c r="A4" s="21"/>
-      <c r="B4" s="309"/>
-      <c r="C4" s="309"/>
-      <c r="D4" s="309"/>
-      <c r="E4" s="309"/>
-      <c r="F4" s="309"/>
-      <c r="G4" s="309"/>
-      <c r="H4" s="309"/>
-      <c r="I4" s="309"/>
-      <c r="J4" s="309"/>
-      <c r="K4" s="309"/>
-      <c r="L4" s="309"/>
-      <c r="M4" s="309"/>
-      <c r="N4" s="309"/>
-      <c r="O4" s="309"/>
-      <c r="P4" s="309"/>
-      <c r="Q4" s="309"/>
-      <c r="R4" s="309"/>
-      <c r="S4" s="309"/>
-      <c r="T4" s="309"/>
-      <c r="U4" s="309"/>
+      <c r="B4" s="324"/>
+      <c r="C4" s="324"/>
+      <c r="D4" s="324"/>
+      <c r="E4" s="324"/>
+      <c r="F4" s="324"/>
+      <c r="G4" s="324"/>
+      <c r="H4" s="324"/>
+      <c r="I4" s="324"/>
+      <c r="J4" s="324"/>
+      <c r="K4" s="324"/>
+      <c r="L4" s="324"/>
+      <c r="M4" s="324"/>
+      <c r="N4" s="324"/>
+      <c r="O4" s="324"/>
+      <c r="P4" s="324"/>
+      <c r="Q4" s="324"/>
+      <c r="R4" s="324"/>
+      <c r="S4" s="324"/>
+      <c r="T4" s="324"/>
+      <c r="U4" s="324"/>
       <c r="V4" s="152"/>
       <c r="W4" s="22"/>
       <c r="X4" s="22"/>
@@ -4391,13 +4391,13 @@
     <row r="7" spans="1:36" s="31" customFormat="1" ht="35.25" customHeight="1">
       <c r="A7" s="26"/>
       <c r="B7" s="26"/>
-      <c r="C7" s="301"/>
-      <c r="D7" s="302"/>
-      <c r="E7" s="302"/>
-      <c r="F7" s="302"/>
-      <c r="G7" s="302"/>
-      <c r="H7" s="302"/>
-      <c r="I7" s="302"/>
+      <c r="C7" s="325"/>
+      <c r="D7" s="326"/>
+      <c r="E7" s="326"/>
+      <c r="F7" s="326"/>
+      <c r="G7" s="326"/>
+      <c r="H7" s="326"/>
+      <c r="I7" s="326"/>
       <c r="J7" s="153"/>
       <c r="K7" s="30"/>
       <c r="N7" s="32"/>
@@ -4411,10 +4411,10 @@
       <c r="V7" s="46"/>
       <c r="W7" s="47"/>
       <c r="X7" s="47"/>
-      <c r="Y7" s="303" t="s">
+      <c r="Y7" s="327" t="s">
         <v>6</v>
       </c>
-      <c r="Z7" s="303"/>
+      <c r="Z7" s="327"/>
       <c r="AA7" s="48"/>
       <c r="AB7" s="49"/>
       <c r="AC7" s="38"/>
@@ -4422,7 +4422,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AF7" s="301" t="str">
+      <c r="AF7" s="325" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">Ký hiệu viết tắt: 
 TR: Test Report
@@ -4430,7 +4430,7 @@
 NA: Not applicable
 </v>
       </c>
-      <c r="AG7" s="303" t="str">
+      <c r="AG7" s="327" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4470,8 +4470,8 @@
       <c r="V8" s="40"/>
       <c r="W8" s="51"/>
       <c r="X8" s="33"/>
-      <c r="Y8" s="303"/>
-      <c r="Z8" s="303"/>
+      <c r="Y8" s="327"/>
+      <c r="Z8" s="327"/>
       <c r="AA8" s="48"/>
       <c r="AB8" s="49"/>
       <c r="AC8" s="38"/>
@@ -4479,11 +4479,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AF8" s="301" t="str">
+      <c r="AF8" s="325" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AG8" s="303" t="str">
+      <c r="AG8" s="327" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4675,10 +4675,10 @@
     </row>
     <row r="13" spans="1:36" s="31" customFormat="1" ht="50" customHeight="1">
       <c r="A13" s="26"/>
-      <c r="B13" s="319">
+      <c r="B13" s="310">
         <v>20143</v>
       </c>
-      <c r="C13" s="322" t="s">
+      <c r="C13" s="313" t="s">
         <v>240</v>
       </c>
       <c r="D13" s="297" t="s">
@@ -4687,19 +4687,19 @@
       <c r="E13" s="203">
         <v>10603496</v>
       </c>
-      <c r="F13" s="325" t="s">
+      <c r="F13" s="316" t="s">
         <v>397</v>
       </c>
-      <c r="G13" s="325" t="s">
+      <c r="G13" s="316" t="s">
         <v>399</v>
       </c>
-      <c r="H13" s="325" t="s">
+      <c r="H13" s="316" t="s">
         <v>398</v>
       </c>
-      <c r="I13" s="310">
+      <c r="I13" s="301">
         <v>2</v>
       </c>
-      <c r="J13" s="313">
+      <c r="J13" s="304">
         <v>45968</v>
       </c>
       <c r="K13" s="34"/>
@@ -4725,19 +4725,19 @@
     </row>
     <row r="14" spans="1:36" s="31" customFormat="1" ht="50" customHeight="1">
       <c r="A14" s="26"/>
-      <c r="B14" s="320"/>
-      <c r="C14" s="323"/>
+      <c r="B14" s="311"/>
+      <c r="C14" s="314"/>
       <c r="D14" s="297" t="s">
         <v>394</v>
       </c>
       <c r="E14" s="203" t="s">
         <v>384</v>
       </c>
-      <c r="F14" s="326"/>
-      <c r="G14" s="326"/>
-      <c r="H14" s="326"/>
-      <c r="I14" s="311"/>
-      <c r="J14" s="314"/>
+      <c r="F14" s="317"/>
+      <c r="G14" s="317"/>
+      <c r="H14" s="317"/>
+      <c r="I14" s="302"/>
+      <c r="J14" s="305"/>
       <c r="K14" s="30"/>
       <c r="L14" s="34"/>
       <c r="M14" s="34"/>
@@ -4762,15 +4762,15 @@
     </row>
     <row r="15" spans="1:36" s="31" customFormat="1" ht="50" customHeight="1">
       <c r="A15" s="26"/>
-      <c r="B15" s="321"/>
-      <c r="C15" s="324"/>
+      <c r="B15" s="312"/>
+      <c r="C15" s="315"/>
       <c r="D15" s="297"/>
       <c r="E15" s="203"/>
-      <c r="F15" s="327"/>
-      <c r="G15" s="327"/>
-      <c r="H15" s="327"/>
-      <c r="I15" s="312"/>
-      <c r="J15" s="315"/>
+      <c r="F15" s="318"/>
+      <c r="G15" s="318"/>
+      <c r="H15" s="318"/>
+      <c r="I15" s="303"/>
+      <c r="J15" s="306"/>
       <c r="K15" s="30"/>
       <c r="L15" s="34"/>
       <c r="M15" s="34"/>
@@ -4890,23 +4890,23 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AI17" s="317" t="s">
+      <c r="AI17" s="308" t="s">
         <v>18</v>
       </c>
-      <c r="AJ17" s="318"/>
+      <c r="AJ17" s="309"/>
     </row>
     <row r="18" spans="1:36" ht="43.5" customHeight="1">
-      <c r="A18" s="316" t="s">
+      <c r="A18" s="307" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="316"/>
-      <c r="C18" s="316"/>
-      <c r="D18" s="316"/>
-      <c r="E18" s="316"/>
-      <c r="F18" s="316"/>
-      <c r="G18" s="316"/>
-      <c r="H18" s="316"/>
-      <c r="I18" s="316"/>
+      <c r="B18" s="307"/>
+      <c r="C18" s="307"/>
+      <c r="D18" s="307"/>
+      <c r="E18" s="307"/>
+      <c r="F18" s="307"/>
+      <c r="G18" s="307"/>
+      <c r="H18" s="307"/>
+      <c r="I18" s="307"/>
       <c r="J18" s="61"/>
       <c r="K18" s="189"/>
       <c r="L18" s="63" t="s">
@@ -5402,6 +5402,16 @@
   </sheetData>
   <sheetProtection sort="0" autoFilter="0"/>
   <mergeCells count="19">
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="Z7:Z8"/>
+    <mergeCell ref="AF7:AF8"/>
+    <mergeCell ref="AG7:AG8"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="B3:U4"/>
     <mergeCell ref="I13:I15"/>
     <mergeCell ref="J13:J15"/>
     <mergeCell ref="A18:I18"/>
@@ -5411,16 +5421,6 @@
     <mergeCell ref="F13:F15"/>
     <mergeCell ref="G13:G15"/>
     <mergeCell ref="H13:H15"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="B3:U4"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="Z7:Z8"/>
-    <mergeCell ref="AF7:AF8"/>
-    <mergeCell ref="AG7:AG8"/>
   </mergeCells>
   <conditionalFormatting sqref="W1:W11 V12:V13 W14:W19 W21:W1048576">
     <cfRule type="notContainsBlanks" dxfId="28" priority="2">
@@ -5444,7 +5444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AN316"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="82" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="82" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A12" sqref="A12"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
@@ -5524,10 +5524,10 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="5"/>
       <c r="AA1" s="2"/>
-      <c r="AB1" s="304" t="s">
+      <c r="AB1" s="319" t="s">
         <v>1</v>
       </c>
-      <c r="AC1" s="305"/>
+      <c r="AC1" s="320"/>
       <c r="AD1" s="6"/>
       <c r="AE1" s="6"/>
       <c r="AF1" s="7"/>
@@ -5535,11 +5535,11 @@
         <f t="shared" ref="AH1:AM20" si="0">IF(AA1&lt;&gt;"",AA1,"")</f>
         <v/>
       </c>
-      <c r="AI1" s="304" t="str">
+      <c r="AI1" s="319" t="str">
         <f t="shared" si="0"/>
         <v>Mã số: BM-KĐ-14</v>
       </c>
-      <c r="AJ1" s="305" t="str">
+      <c r="AJ1" s="320" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -5584,10 +5584,10 @@
       <c r="Y2" s="13"/>
       <c r="Z2" s="14"/>
       <c r="AA2" s="11"/>
-      <c r="AB2" s="306" t="s">
+      <c r="AB2" s="321" t="s">
         <v>2</v>
       </c>
-      <c r="AC2" s="307"/>
+      <c r="AC2" s="322"/>
       <c r="AD2" s="15"/>
       <c r="AE2" s="15"/>
       <c r="AF2" s="7"/>
@@ -5595,11 +5595,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AI2" s="306" t="str">
+      <c r="AI2" s="321" t="str">
         <f t="shared" si="0"/>
         <v>Ngày ban hành: 01/7/2015</v>
       </c>
-      <c r="AJ2" s="307" t="str">
+      <c r="AJ2" s="322" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -5620,29 +5620,29 @@
       <c r="A3" s="156"/>
       <c r="B3" s="268"/>
       <c r="C3" s="268"/>
-      <c r="D3" s="308" t="s">
+      <c r="D3" s="323" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="308"/>
-      <c r="F3" s="308"/>
-      <c r="G3" s="308"/>
-      <c r="H3" s="308"/>
-      <c r="I3" s="308"/>
-      <c r="J3" s="308"/>
-      <c r="K3" s="308"/>
-      <c r="L3" s="308"/>
-      <c r="M3" s="308"/>
-      <c r="N3" s="308"/>
-      <c r="O3" s="308"/>
-      <c r="P3" s="308"/>
-      <c r="Q3" s="344"/>
-      <c r="R3" s="308"/>
-      <c r="S3" s="308"/>
-      <c r="T3" s="308"/>
-      <c r="U3" s="308"/>
-      <c r="V3" s="308"/>
-      <c r="W3" s="308"/>
-      <c r="X3" s="308"/>
+      <c r="E3" s="323"/>
+      <c r="F3" s="323"/>
+      <c r="G3" s="323"/>
+      <c r="H3" s="323"/>
+      <c r="I3" s="323"/>
+      <c r="J3" s="323"/>
+      <c r="K3" s="323"/>
+      <c r="L3" s="323"/>
+      <c r="M3" s="323"/>
+      <c r="N3" s="323"/>
+      <c r="O3" s="323"/>
+      <c r="P3" s="323"/>
+      <c r="Q3" s="328"/>
+      <c r="R3" s="323"/>
+      <c r="S3" s="323"/>
+      <c r="T3" s="323"/>
+      <c r="U3" s="323"/>
+      <c r="V3" s="323"/>
+      <c r="W3" s="323"/>
+      <c r="X3" s="323"/>
       <c r="Y3" s="151"/>
       <c r="Z3" s="17"/>
       <c r="AA3" s="18"/>
@@ -5682,27 +5682,27 @@
       <c r="A4" s="157"/>
       <c r="B4" s="269"/>
       <c r="C4" s="269"/>
-      <c r="D4" s="309"/>
-      <c r="E4" s="309"/>
-      <c r="F4" s="309"/>
-      <c r="G4" s="309"/>
-      <c r="H4" s="309"/>
-      <c r="I4" s="309"/>
-      <c r="J4" s="309"/>
-      <c r="K4" s="309"/>
-      <c r="L4" s="309"/>
-      <c r="M4" s="309"/>
-      <c r="N4" s="309"/>
-      <c r="O4" s="309"/>
-      <c r="P4" s="309"/>
-      <c r="Q4" s="345"/>
-      <c r="R4" s="309"/>
-      <c r="S4" s="309"/>
-      <c r="T4" s="309"/>
-      <c r="U4" s="309"/>
-      <c r="V4" s="309"/>
-      <c r="W4" s="309"/>
-      <c r="X4" s="309"/>
+      <c r="D4" s="324"/>
+      <c r="E4" s="324"/>
+      <c r="F4" s="324"/>
+      <c r="G4" s="324"/>
+      <c r="H4" s="324"/>
+      <c r="I4" s="324"/>
+      <c r="J4" s="324"/>
+      <c r="K4" s="324"/>
+      <c r="L4" s="324"/>
+      <c r="M4" s="324"/>
+      <c r="N4" s="324"/>
+      <c r="O4" s="324"/>
+      <c r="P4" s="324"/>
+      <c r="Q4" s="329"/>
+      <c r="R4" s="324"/>
+      <c r="S4" s="324"/>
+      <c r="T4" s="324"/>
+      <c r="U4" s="324"/>
+      <c r="V4" s="324"/>
+      <c r="W4" s="324"/>
+      <c r="X4" s="324"/>
       <c r="Y4" s="152"/>
       <c r="Z4" s="22"/>
       <c r="AA4" s="22"/>
@@ -5853,14 +5853,14 @@
       <c r="B7" s="158"/>
       <c r="C7" s="158"/>
       <c r="D7" s="26"/>
-      <c r="E7" s="301"/>
-      <c r="F7" s="302"/>
-      <c r="G7" s="302"/>
-      <c r="H7" s="302"/>
-      <c r="I7" s="302"/>
-      <c r="J7" s="302"/>
-      <c r="K7" s="302"/>
-      <c r="L7" s="302"/>
+      <c r="E7" s="325"/>
+      <c r="F7" s="326"/>
+      <c r="G7" s="326"/>
+      <c r="H7" s="326"/>
+      <c r="I7" s="326"/>
+      <c r="J7" s="326"/>
+      <c r="K7" s="326"/>
+      <c r="L7" s="326"/>
       <c r="M7" s="153"/>
       <c r="N7" s="30"/>
       <c r="Q7" s="171"/>
@@ -5874,10 +5874,10 @@
       <c r="Y7" s="46"/>
       <c r="Z7" s="47"/>
       <c r="AA7" s="47"/>
-      <c r="AB7" s="303" t="s">
+      <c r="AB7" s="327" t="s">
         <v>221</v>
       </c>
-      <c r="AC7" s="303"/>
+      <c r="AC7" s="327"/>
       <c r="AD7" s="48"/>
       <c r="AE7" s="49"/>
       <c r="AF7" s="38"/>
@@ -5885,7 +5885,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AI7" s="301" t="str">
+      <c r="AI7" s="325" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">Ký hiệu viết tắt: 
 TR: Test Report
@@ -5894,7 +5894,7 @@
 SDS: Safety Data Sheet
 </v>
       </c>
-      <c r="AJ7" s="303" t="str">
+      <c r="AJ7" s="327" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -5941,8 +5941,8 @@
       <c r="Y8" s="40"/>
       <c r="Z8" s="51"/>
       <c r="AA8" s="33"/>
-      <c r="AB8" s="303"/>
-      <c r="AC8" s="303"/>
+      <c r="AB8" s="327"/>
+      <c r="AC8" s="327"/>
       <c r="AD8" s="48"/>
       <c r="AE8" s="49"/>
       <c r="AF8" s="38"/>
@@ -5950,11 +5950,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AI8" s="301" t="str">
+      <c r="AI8" s="325" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AJ8" s="303" t="str">
+      <c r="AJ8" s="327" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -6158,10 +6158,10 @@
     </row>
     <row r="13" spans="1:39" s="31" customFormat="1" ht="52.5" customHeight="1">
       <c r="A13" s="158"/>
-      <c r="B13" s="338">
+      <c r="B13" s="340">
         <v>20143</v>
       </c>
-      <c r="C13" s="335" t="s">
+      <c r="C13" s="337" t="s">
         <v>240</v>
       </c>
       <c r="D13" s="271" t="s">
@@ -6170,16 +6170,16 @@
       <c r="E13" s="270">
         <v>10603496</v>
       </c>
-      <c r="F13" s="341" t="s">
+      <c r="F13" s="343" t="s">
         <v>237</v>
       </c>
       <c r="G13" s="264"/>
       <c r="H13" s="264"/>
       <c r="I13" s="264"/>
-      <c r="J13" s="328">
+      <c r="J13" s="330">
         <v>2</v>
       </c>
-      <c r="K13" s="332">
+      <c r="K13" s="334">
         <v>45968</v>
       </c>
       <c r="O13" s="34"/>
@@ -6205,22 +6205,22 @@
     </row>
     <row r="14" spans="1:39" s="31" customFormat="1" ht="52.5" customHeight="1">
       <c r="A14" s="158"/>
-      <c r="B14" s="339"/>
-      <c r="C14" s="336"/>
+      <c r="B14" s="341"/>
+      <c r="C14" s="338"/>
       <c r="D14" s="271" t="s">
         <v>394</v>
       </c>
       <c r="E14" s="270" t="s">
         <v>384</v>
       </c>
-      <c r="F14" s="342"/>
+      <c r="F14" s="344"/>
       <c r="G14" s="298" t="s">
         <v>397</v>
       </c>
       <c r="H14" s="265"/>
       <c r="I14" s="265"/>
-      <c r="J14" s="329"/>
-      <c r="K14" s="333"/>
+      <c r="J14" s="331"/>
+      <c r="K14" s="335"/>
       <c r="O14" s="34"/>
       <c r="P14" s="34"/>
       <c r="Q14" s="172"/>
@@ -6244,16 +6244,16 @@
     </row>
     <row r="15" spans="1:39" s="31" customFormat="1" ht="52.5" customHeight="1">
       <c r="A15" s="158"/>
-      <c r="B15" s="340"/>
-      <c r="C15" s="337"/>
+      <c r="B15" s="342"/>
+      <c r="C15" s="339"/>
       <c r="D15" s="271"/>
       <c r="E15" s="270"/>
-      <c r="F15" s="343"/>
+      <c r="F15" s="345"/>
       <c r="G15" s="266"/>
       <c r="H15" s="266"/>
       <c r="I15" s="266"/>
-      <c r="J15" s="330"/>
-      <c r="K15" s="334"/>
+      <c r="J15" s="332"/>
+      <c r="K15" s="336"/>
       <c r="O15" s="34"/>
       <c r="P15" s="34"/>
       <c r="Q15" s="172"/>
@@ -6414,26 +6414,26 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AL18" s="317" t="s">
+      <c r="AL18" s="308" t="s">
         <v>18</v>
       </c>
-      <c r="AM18" s="318"/>
+      <c r="AM18" s="309"/>
     </row>
     <row r="19" spans="1:39" ht="44.5" customHeight="1">
-      <c r="A19" s="331" t="s">
+      <c r="A19" s="333" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="331"/>
-      <c r="C19" s="331"/>
-      <c r="D19" s="316"/>
-      <c r="E19" s="316"/>
-      <c r="F19" s="316"/>
-      <c r="G19" s="316"/>
-      <c r="H19" s="316"/>
-      <c r="I19" s="316"/>
-      <c r="J19" s="316"/>
-      <c r="K19" s="316"/>
-      <c r="L19" s="316"/>
+      <c r="B19" s="333"/>
+      <c r="C19" s="333"/>
+      <c r="D19" s="307"/>
+      <c r="E19" s="307"/>
+      <c r="F19" s="307"/>
+      <c r="G19" s="307"/>
+      <c r="H19" s="307"/>
+      <c r="I19" s="307"/>
+      <c r="J19" s="307"/>
+      <c r="K19" s="307"/>
+      <c r="L19" s="307"/>
       <c r="M19" s="61"/>
       <c r="N19" s="62"/>
       <c r="O19" s="63" t="s">
@@ -28425,16 +28425,6 @@
   </sheetData>
   <sheetProtection sort="0" autoFilter="0"/>
   <mergeCells count="17">
-    <mergeCell ref="E7:L7"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="AC7:AC8"/>
-    <mergeCell ref="AI7:AI8"/>
-    <mergeCell ref="AJ7:AJ8"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AI1:AJ1"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="D3:X4"/>
     <mergeCell ref="J13:J15"/>
     <mergeCell ref="AL18:AM18"/>
     <mergeCell ref="A19:L19"/>
@@ -28442,6 +28432,16 @@
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="F13:F15"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AI1:AJ1"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="D3:X4"/>
+    <mergeCell ref="E7:L7"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="AC7:AC8"/>
+    <mergeCell ref="AI7:AI8"/>
+    <mergeCell ref="AJ7:AJ8"/>
   </mergeCells>
   <conditionalFormatting sqref="Z34:Z38">
     <cfRule type="notContainsBlanks" dxfId="27" priority="50">

</xml_diff>